<commit_message>
+Question_2 completed -Annotations pending
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rencita.Monteiro\Documents\UiPath\Rencita_Day_10_Assingment_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97742415-6B38-46AD-951F-338DFD73A8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE7C15B-276C-4496-8EFC-103F3EB73194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -163,13 +163,46 @@
   </si>
   <si>
     <t>Assignment_1</t>
+  </si>
+  <si>
+    <t>OutputWorkbookPath</t>
+  </si>
+  <si>
+    <t>Data/Output/Assignment1.xlsx</t>
+  </si>
+  <si>
+    <t>OutputSheetName</t>
+  </si>
+  <si>
+    <t>NSE</t>
+  </si>
+  <si>
+    <t>BrowserPath</t>
+  </si>
+  <si>
+    <t>https://www.nseindia.com/</t>
+  </si>
+  <si>
+    <t>NSEBrowserPath</t>
+  </si>
+  <si>
+    <t>https://www.nseindia.com/get-quotes/equity?symbol=</t>
+  </si>
+  <si>
+    <t>MailCredentials</t>
+  </si>
+  <si>
+    <t>MailCredentails</t>
+  </si>
+  <si>
+    <t>ToMailAddress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +226,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,10 +250,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -224,8 +264,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,7 +583,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -620,7 +662,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1624,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1806,10 +1855,38 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2779,6 +2856,10 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{1001B93F-5B22-469A-9688-EDA4F9592305}"/>
+    <hyperlink ref="B21" r:id="rId2" xr:uid="{625C3645-7809-43FA-9657-1BA14E887335}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2787,7 +2868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2833,7 +2916,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>